<commit_message>
lesson plans added till week06 to it security
</commit_message>
<xml_diff>
--- a/docs/projects/IT Security órák/Terv.xlsx
+++ b/docs/projects/IT Security órák/Terv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\digitalis_kultura\docs\projects\IT Security órák\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8CE61B8-3C04-4310-9F22-E5D173AB2260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0668A01A-A868-40BB-8658-A6D67FCA0BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
   <si>
     <t>Week01</t>
   </si>
@@ -94,6 +94,33 @@
   </si>
   <si>
     <t>bluetooth vs wifi</t>
+  </si>
+  <si>
+    <t>Mi az az internet 2?</t>
+  </si>
+  <si>
+    <t>Free wifi veszélyei.</t>
+  </si>
+  <si>
+    <t>Jelszókezelés, jelszó feltörések(databreaches)</t>
+  </si>
+  <si>
+    <t>Email spam, phising, data theft, blackmail</t>
+  </si>
+  <si>
+    <t>Mi az az email, internetes levelezés.</t>
+  </si>
+  <si>
+    <t>Jelszavak, kódolások működése, titkosítás alapjai</t>
+  </si>
+  <si>
+    <t>Kvantumszámítógépek, titkosítás fontossága</t>
+  </si>
+  <si>
+    <t>Beszélgetős óra - az előző órai dolgokról</t>
+  </si>
+  <si>
+    <t>Week06</t>
   </si>
 </sst>
 </file>
@@ -198,19 +225,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -491,31 +516,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="77" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -531,88 +561,120 @@
       <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K3" s="2"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J5" s="4" t="s">
+      <c r="K4" s="2"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J6" s="4" t="s">
+      <c r="K5" s="2"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J7" s="4" t="s">
+      <c r="K6" s="2"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J8" s="4" t="s">
+      <c r="K7" s="2"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J9" s="4" t="s">
+      <c r="K8" s="2"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J10" s="4" t="s">
+      <c r="K9" s="2"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="J11" s="4" t="s">
+      <c r="K10" s="2"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J12" s="4" t="s">
+      <c r="K11" s="2"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="K12" s="5"/>
-    </row>
-    <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J13" s="7" t="s">
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J13" s="3" t="s">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
it sec lesson update
</commit_message>
<xml_diff>
--- a/docs/projects/IT Security órák/Terv.xlsx
+++ b/docs/projects/IT Security órák/Terv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\digitalis_kultura\docs\projects\IT Security órák\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0668A01A-A868-40BB-8658-A6D67FCA0BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E71C1F-5662-41F2-91CC-4A2F2AD1FDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>IT Security - Internet biztonság</t>
   </si>
   <si>
-    <t>Lesson01 - Mi az a wifi?</t>
-  </si>
-  <si>
     <t>UTP kábel mint adatátviteli közeg</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>rádióhullámok</t>
   </si>
   <si>
-    <t>különböző frekvencia(fontos hogy ne legyen interferencia, pl emergency services)ú</t>
-  </si>
-  <si>
     <t>2.4ghz és 5ghz - unlicensed</t>
   </si>
   <si>
@@ -90,9 +84,6 @@
     <t>Mi az az internet?</t>
   </si>
   <si>
-    <t>Lesson02 - Mi az az internet?</t>
-  </si>
-  <si>
     <t>bluetooth vs wifi</t>
   </si>
   <si>
@@ -121,6 +112,15 @@
   </si>
   <si>
     <t>Week06</t>
+  </si>
+  <si>
+    <t>különböző frekvencia(fontos hogy ne legyen interferencia, pl emergency services)</t>
+  </si>
+  <si>
+    <t>Lesson03 - Mi az a wifi?</t>
+  </si>
+  <si>
+    <t>Lesson0102 - Mi az az internet?</t>
   </si>
 </sst>
 </file>
@@ -518,20 +518,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="77" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -562,13 +562,13 @@
         <v>4</v>
       </c>
       <c r="G2" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -576,25 +576,25 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>23</v>
-      </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K3" s="2"/>
     </row>
@@ -606,77 +606,78 @@
         <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="G4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J5" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J6" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J8" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J9" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K9" s="2"/>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J10" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="K10" s="2"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J12" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K12" s="3"/>
+        <v>17</v>
+      </c>
+      <c r="K12" s="2"/>
     </row>
     <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="J13" s="3" t="s">
-        <v>22</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="K13" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
week01 of IT security presentation finished
</commit_message>
<xml_diff>
--- a/docs/projects/IT Security órák/Terv.xlsx
+++ b/docs/projects/IT Security órák/Terv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\digitalis_kultura\docs\projects\IT Security órák\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E71C1F-5662-41F2-91CC-4A2F2AD1FDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013AF247-DD3A-4CAF-845E-656A6272435F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Week01</t>
   </si>
@@ -120,7 +120,73 @@
     <t>Lesson03 - Mi az a wifi?</t>
   </si>
   <si>
-    <t>Lesson0102 - Mi az az internet?</t>
+    <t>Lesson01 - Mi az az internet?</t>
+  </si>
+  <si>
+    <t>Lesson02 - Mi az az internet 2?</t>
+  </si>
+  <si>
+    <t>Mi az a MAC cím = DNS az embernél.</t>
+  </si>
+  <si>
+    <t>IP címek - ipv4 minta, ipv6 minta</t>
+  </si>
+  <si>
+    <t>Kezdete - arpanet</t>
+  </si>
+  <si>
+    <t>Egyetemi hálózat - &gt; világháló</t>
+  </si>
+  <si>
+    <t>Lényege régen vs. Ma</t>
+  </si>
+  <si>
+    <t>Földi összeköttetések - Atlanti kábel, ausztrália kábel</t>
+  </si>
+  <si>
+    <t>Műholdas összeköttetések - Starlink</t>
+  </si>
+  <si>
+    <t>WWW - World Wide Web</t>
+  </si>
+  <si>
+    <t>Computer network types - NFC, PAN, LAN, WLAN, WAN, MAN, INTERNET</t>
+  </si>
+  <si>
+    <t>Internetet használó eszközök ma</t>
+  </si>
+  <si>
+    <t>Hány darab eszköz van ami tud csatlakozni az internetre kb</t>
+  </si>
+  <si>
+    <t>Lesson04 - Áttekintés</t>
+  </si>
+  <si>
+    <t>Lesson05 - Email, internetes levelezés</t>
+  </si>
+  <si>
+    <t>Lesson06 - Email átverések, spam, phising, blackmail, data theft</t>
+  </si>
+  <si>
+    <t>Lesson07 - Free wifi veszélyei</t>
+  </si>
+  <si>
+    <t>Lesson08 - Áttekintés</t>
+  </si>
+  <si>
+    <t>Lesson09 - Jelszavak működése, titkosítás alapok</t>
+  </si>
+  <si>
+    <t>Lesson10 - Jelszókezelés, jelszavak feltörése/megszerzése</t>
+  </si>
+  <si>
+    <t>Lesson11 - Kvantumszámítógépek, a jövő gépei, titkosításai</t>
+  </si>
+  <si>
+    <t>Lesson12 - Áttekintés</t>
+  </si>
+  <si>
+    <t>Lesson13</t>
   </si>
 </sst>
 </file>
@@ -516,25 +582,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="45.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="41" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="75.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="77" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>8</v>
       </c>
@@ -544,7 +608,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>0</v>
@@ -564,14 +628,8 @@
       <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -593,12 +651,8 @@
       <c r="G3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K3" s="2"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -620,64 +674,281 @@
       <c r="G4" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="2" t="s">
+    </row>
+    <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="2"/>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J5" s="2" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="2"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J6" s="2" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J7" s="2" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="2"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J8" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K8" s="2"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J9" s="2" t="s">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="2"/>
+      <c r="C13" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J10" s="2" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="2"/>
+      <c r="C14" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J11" s="2" t="s">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="2"/>
+      <c r="C15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J12" s="2" t="s">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="2"/>
+      <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="J13" s="3" t="s">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K13" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+    </row>
+    <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
more topics added to IT security lessons as ideas, higher level word added to class 9
</commit_message>
<xml_diff>
--- a/docs/projects/IT Security órák/Terv.xlsx
+++ b/docs/projects/IT Security órák/Terv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\digitalis_kultura\docs\projects\IT Security órák\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jooan\Documents\GitHub Projects\digitalis_kultura\docs\projects\IT Security órák\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{013AF247-DD3A-4CAF-845E-656A6272435F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F685249F-F2E6-4490-9C6F-B1644238B099}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="56">
   <si>
     <t>Week01</t>
   </si>
@@ -187,6 +187,12 @@
   </si>
   <si>
     <t>Lesson13</t>
+  </si>
+  <si>
+    <t>Orosz hackerek, etikus hackerek</t>
+  </si>
+  <si>
+    <t>Amerikai srác aki feltörte a Pentagont</t>
   </si>
 </sst>
 </file>
@@ -584,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,6 +657,9 @@
       <c r="G3" t="s">
         <v>26</v>
       </c>
+      <c r="H3" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -673,6 +682,9 @@
       </c>
       <c r="G4" t="s">
         <v>27</v>
+      </c>
+      <c r="H4" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
it sec excel updated, example email added
</commit_message>
<xml_diff>
--- a/docs/projects/IT Security órák/Terv.xlsx
+++ b/docs/projects/IT Security órák/Terv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\digitalis_kultura\docs\projects\IT Security órák\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jooan\Documents\GitHub Projects\digitalis_kultura\docs\projects\IT Security órák\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F1CB33-1F97-450E-B108-5F07582CA763}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F932EF5C-61B1-47F6-A2AE-B9FF46078588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
   <si>
     <t>Week01</t>
   </si>
@@ -220,6 +220,33 @@
   </si>
   <si>
     <t>Magyar találmányok a világban</t>
+  </si>
+  <si>
+    <t>Emailes veszélyek</t>
+  </si>
+  <si>
+    <t>Email phising gyakori kinézete</t>
+  </si>
+  <si>
+    <t>Hogyan ismerjük fel ezeket a veszélyeket</t>
+  </si>
+  <si>
+    <t>Email spam gyakori kinézete</t>
+  </si>
+  <si>
+    <t>Phising weboldal példa</t>
+  </si>
+  <si>
+    <t>Hogyan védekezzünk - "Józan paraszti ész használata", "semmi sincs ingyen"</t>
+  </si>
+  <si>
+    <t>Mire tudják felhasználni az adatainkat, ha megszerzik</t>
+  </si>
+  <si>
+    <t>Free wifi - dejó hogy van de elmondani miért veszélyes</t>
+  </si>
+  <si>
+    <t>Példa arra miért veszélyes, hogyan tudnak átverni/meglopni ezzel</t>
   </si>
 </sst>
 </file>
@@ -324,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -335,6 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -617,14 +645,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="75.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="58.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="77" bestFit="1" customWidth="1"/>
@@ -752,7 +780,9 @@
       <c r="D7" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>72</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -767,7 +797,9 @@
       <c r="D8" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -912,7 +944,9 @@
         <v>41</v>
       </c>
       <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="D19" s="2" t="s">
+        <v>65</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -922,7 +956,9 @@
         <v>34</v>
       </c>
       <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="D20" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
@@ -932,7 +968,9 @@
         <v>33</v>
       </c>
       <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="D21" s="6" t="s">
+        <v>68</v>
+      </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -942,7 +980,9 @@
         <v>42</v>
       </c>
       <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -952,7 +992,9 @@
         <v>43</v>
       </c>
       <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="D23" s="6" t="s">
+        <v>69</v>
+      </c>
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -962,7 +1004,9 @@
         <v>63</v>
       </c>
       <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>70</v>
+      </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -970,7 +1014,9 @@
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>71</v>
+      </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>

</xml_diff>

<commit_message>
it sec excel plann fully planned - ver1
</commit_message>
<xml_diff>
--- a/docs/projects/IT Security órák/Terv.xlsx
+++ b/docs/projects/IT Security órák/Terv.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jooan\Documents\GitHub Projects\digitalis_kultura\docs\projects\IT Security órák\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F932EF5C-61B1-47F6-A2AE-B9FF46078588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7AD656-3476-4176-AAB3-49ED2BED38CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
   <si>
     <t>Week01</t>
   </si>
@@ -247,6 +247,66 @@
   </si>
   <si>
     <t>Példa arra miért veszélyes, hogyan tudnak átverni/meglopni ezzel</t>
+  </si>
+  <si>
+    <t>Érdekes történetek az IT világából</t>
+  </si>
+  <si>
+    <t>Orosz hackerek (legalitás, játék feltörők, rendszer hackerek)</t>
+  </si>
+  <si>
+    <t>Amerikai hackerek (legalitás, pentagont feltörő srác)</t>
+  </si>
+  <si>
+    <t>USA - Orosz különbségek hackererk, kíbervédelem</t>
+  </si>
+  <si>
+    <t>Lehetséges témák?</t>
+  </si>
+  <si>
+    <t>Magyar találmányok</t>
+  </si>
+  <si>
+    <t>Mi az a kavntumszámítógép?</t>
+  </si>
+  <si>
+    <t>Mire lehet használni?</t>
+  </si>
+  <si>
+    <t>Miben más a mostani pc-k től</t>
+  </si>
+  <si>
+    <t>Miért jó is meg rossz is? - Feltörtések, számítási kapacitás</t>
+  </si>
+  <si>
+    <t>Jelszavak régen, kémek, miért kellett már régen is használni</t>
+  </si>
+  <si>
+    <t>Titkosítások lényege, enigma + feltörésének története</t>
+  </si>
+  <si>
+    <t>Komolyabb titkosítások létrejötte</t>
+  </si>
+  <si>
+    <t>Néhány példa a multból (ceaser)</t>
+  </si>
+  <si>
+    <t>Modern titkosítások (sha256, base64, stb.)</t>
+  </si>
+  <si>
+    <t>Jelszókezelés manapság</t>
+  </si>
+  <si>
+    <t>Jelszókezelő appok ( lastpass, bitwarden) - fizetős-ingyenes</t>
+  </si>
+  <si>
+    <t>Miért jó mindenhova más jelszót használni</t>
+  </si>
+  <si>
+    <t>Mit tudnak kezdeni a jelszavunkkal ha megszerzik</t>
+  </si>
+  <si>
+    <t>2-factor auth fontossága</t>
   </si>
 </sst>
 </file>
@@ -291,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -347,11 +407,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -360,6 +463,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -645,15 +757,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="75.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="53.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="77" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
@@ -783,9 +896,15 @@
       <c r="E7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
+      <c r="F7" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -800,9 +919,15 @@
       <c r="E8" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
+      <c r="F8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
@@ -815,9 +940,15 @@
         <v>62</v>
       </c>
       <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
+      <c r="F9" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
@@ -830,9 +961,15 @@
         <v>59</v>
       </c>
       <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
+      <c r="F10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -845,7 +982,9 @@
         <v>60</v>
       </c>
       <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2" t="s">
+        <v>88</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
@@ -862,7 +1001,9 @@
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="2"/>
@@ -871,9 +1012,10 @@
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="2"/>
@@ -882,7 +1024,6 @@
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
@@ -893,7 +1034,6 @@
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
@@ -943,121 +1083,134 @@
       <c r="B19" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="6"/>
       <c r="D19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="7"/>
       <c r="D20" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="6" t="s">
+      <c r="C21" s="7"/>
+      <c r="D21" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="7"/>
       <c r="D22" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="2"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="2"/>
-      <c r="D23" s="6" t="s">
+      <c r="C23" s="7"/>
+      <c r="D23" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C24" s="2"/>
+      <c r="C24" s="7"/>
       <c r="D24" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="E24" s="7"/>
+      <c r="F24" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
+      <c r="C25" s="7"/>
       <c r="D25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E25" s="2"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+      <c r="C26" s="7"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
+      <c r="C27" s="7"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="2" t="s">
-        <v>56</v>
-      </c>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
+      <c r="C28" s="7"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
+      <c r="E29" s="8"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="4">
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C19:C29"/>
+    <mergeCell ref="E19:E29"/>
+    <mergeCell ref="G19:G29"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
it sec plan changed, ppt for topic 2 finished, trello exercise added
</commit_message>
<xml_diff>
--- a/docs/projects/IT Security órák/Terv.xlsx
+++ b/docs/projects/IT Security órák/Terv.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jooan\Documents\GitHub Projects\digitalis_kultura\docs\projects\IT Security órák\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\digitalis_kultura\docs\projects\IT Security órák\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7AD656-3476-4176-AAB3-49ED2BED38CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F7177C-E75E-4EB4-A829-38231BDB1D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -201,21 +201,12 @@
     <t>Mi az az email?</t>
   </si>
   <si>
-    <t>Email protkolok, röviden</t>
-  </si>
-  <si>
     <t>Első email valaha elküldve</t>
   </si>
   <si>
-    <t>Email szolgáltatások</t>
-  </si>
-  <si>
     <t>Gmail features</t>
   </si>
   <si>
-    <t>Első email szerverek, weboldalak</t>
-  </si>
-  <si>
     <t>NFC</t>
   </si>
   <si>
@@ -307,6 +298,15 @@
   </si>
   <si>
     <t>2-factor auth fontossága</t>
+  </si>
+  <si>
+    <t>AI Tools - Weblapok</t>
+  </si>
+  <si>
+    <t>Mik azok a sütik a weblapokon</t>
+  </si>
+  <si>
+    <t>Trello bemutatása - Órai feladat: 3-4 fős csapatok, mindenki valamilyen vezető pl:CEO, CFO, COO, CTO - Az általuk készített trelloban minden csapat tag legyen benne és mindenki adjon hozzá feladatokat a képzeletbeli alkalmazottainak. - 10 feladat/ember</t>
   </si>
 </sst>
 </file>
@@ -337,7 +337,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -350,8 +350,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -450,11 +456,24 @@
         <color auto="1"/>
       </diagonal>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -474,7 +493,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -757,16 +786,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="4" width="75.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="57.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="77" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="28.85546875" bestFit="1" customWidth="1"/>
@@ -857,7 +886,7 @@
     </row>
     <row r="5" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="H5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -884,176 +913,154 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="9" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="E7" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="2" t="s">
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B10" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>92</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="H7" s="2" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="2" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="F11" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="G13" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" s="2" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="9"/>
+      <c r="C14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="G14" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="2"/>
-      <c r="C13" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="2"/>
-      <c r="C15" s="2" t="s">
+      <c r="B15" s="9"/>
+      <c r="C15" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="2" t="s">
+      <c r="B16" s="9"/>
+      <c r="C16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="3"/>
-      <c r="C17" s="3" t="s">
+      <c r="B17" s="10"/>
+      <c r="C17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
@@ -1080,126 +1087,130 @@
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="11" t="s">
+        <v>93</v>
+      </c>
       <c r="D19" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="2" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="7"/>
+      <c r="C20" s="12"/>
       <c r="D20" s="2" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="E20" s="7"/>
-      <c r="F20" s="9" t="s">
-        <v>91</v>
+      <c r="F20" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="7"/>
+      <c r="C21" s="12"/>
       <c r="D21" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="E21" s="7"/>
       <c r="F21" s="2" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="7"/>
+      <c r="C22" s="12"/>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="E22" s="7"/>
-      <c r="F22" s="2"/>
+      <c r="F22" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="7"/>
+      <c r="C23" s="12"/>
       <c r="D23" s="2" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="E23" s="7"/>
-      <c r="F23" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" s="7"/>
+      <c r="B24" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="12"/>
       <c r="D24" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="E24" s="7"/>
-      <c r="F24" s="2" t="s">
-        <v>93</v>
-      </c>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="7"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="12"/>
       <c r="D25" s="2" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E25" s="7"/>
       <c r="F25" s="2"/>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="2"/>
+      <c r="B26" s="9"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="2" t="s">
+        <v>66</v>
+      </c>
       <c r="E26" s="7"/>
       <c r="F26" s="2"/>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="2"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="12"/>
+      <c r="D27" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="E27" s="7"/>
       <c r="F27" s="2"/>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="2"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="2" t="s">
+        <v>68</v>
+      </c>
       <c r="E28" s="7"/>
       <c r="F28" s="2"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="3"/>
-      <c r="C29" s="8"/>
+      <c r="B29" s="10"/>
+      <c r="C29" s="13"/>
       <c r="D29" s="3"/>
       <c r="E29" s="8"/>
       <c r="F29" s="3"/>

</xml_diff>

<commit_message>
random lesson contents added
</commit_message>
<xml_diff>
--- a/docs/projects/IT Security órák/Terv.xlsx
+++ b/docs/projects/IT Security órák/Terv.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GithubProjects\digitalis_kultura\docs\projects\IT Security órák\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F7177C-E75E-4EB4-A829-38231BDB1D25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DFF64DD-4131-4DBC-A5CB-A580C052A927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-60" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="98">
   <si>
     <t>Week01</t>
   </si>
@@ -307,6 +307,18 @@
   </si>
   <si>
     <t>Trello bemutatása - Órai feladat: 3-4 fős csapatok, mindenki valamilyen vezető pl:CEO, CFO, COO, CTO - Az általuk készített trelloban minden csapat tag legyen benne és mindenki adjon hozzá feladatokat a képzeletbeli alkalmazottainak. - 10 feladat/ember</t>
+  </si>
+  <si>
+    <t>Random óra</t>
+  </si>
+  <si>
+    <t>ai password cracking speed</t>
+  </si>
+  <si>
+    <t>gmail features - képek</t>
+  </si>
+  <si>
+    <t>websites -archive.org, darebee.com, tinywow.com, edx.org,remove.bg,supercook.com, carrd.co,pixlr.com,pdfdrive.com</t>
   </si>
 </sst>
 </file>
@@ -357,7 +369,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -463,7 +475,20 @@
       <right style="medium">
         <color auto="1"/>
       </right>
-      <top style="dashed">
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
         <color auto="1"/>
       </top>
       <bottom/>
@@ -473,7 +498,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -481,6 +506,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -493,16 +520,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -784,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,14 +836,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -913,10 +947,10 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="5" t="s">
         <v>9</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -933,10 +967,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="9" t="s">
+      <c r="B8" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -953,10 +987,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
@@ -970,10 +1004,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D10" t="s">
@@ -988,10 +1022,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="E11" s="2" t="s">
@@ -1005,10 +1039,10 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E12" s="2"/>
@@ -1017,8 +1051,8 @@
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9" t="s">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5" t="s">
         <v>14</v>
       </c>
       <c r="E13" s="2"/>
@@ -1027,8 +1061,8 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="9"/>
-      <c r="C14" s="9" t="s">
+      <c r="B14" s="5"/>
+      <c r="C14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="E14" s="2"/>
@@ -1038,8 +1072,8 @@
       <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="9"/>
-      <c r="C15" s="9" t="s">
+      <c r="B15" s="5"/>
+      <c r="C15" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E15" s="2"/>
@@ -1047,8 +1081,8 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="9"/>
-      <c r="C16" s="9" t="s">
+      <c r="B16" s="5"/>
+      <c r="C16" s="5" t="s">
         <v>17</v>
       </c>
       <c r="E16" s="2"/>
@@ -1057,8 +1091,8 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10"/>
-      <c r="C17" s="10" t="s">
+      <c r="B17" s="6"/>
+      <c r="C17" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E17" s="3"/>
@@ -1070,7 +1104,7 @@
       <c r="B18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="12" t="s">
         <v>44</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -1086,142 +1120,166 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+    <row r="19" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="14" t="s">
         <v>93</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="6"/>
+      <c r="E19" s="8"/>
       <c r="F19" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G19" s="6" t="s">
+      <c r="G19" s="8" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="12"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E20" s="7"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G20" s="7"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="12"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E21" s="7"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G21" s="7"/>
+      <c r="G21" s="9"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C22" s="12"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="7"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G22" s="7"/>
+      <c r="G22" s="9"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C23" s="12"/>
+      <c r="C23" s="11"/>
       <c r="D23" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="E23" s="9"/>
+      <c r="G23" s="9"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C24" s="12"/>
+      <c r="C24" s="11"/>
       <c r="D24" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="G24" s="7"/>
+      <c r="E24" s="9"/>
+      <c r="G24" s="9"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="12"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="11"/>
       <c r="D25" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E25" s="7"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="2"/>
-      <c r="G25" s="7"/>
+      <c r="G25" s="9"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="12"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="11"/>
       <c r="D26" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E26" s="7"/>
+      <c r="E26" s="9"/>
       <c r="F26" s="2"/>
-      <c r="G26" s="7"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="12"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="11"/>
       <c r="D27" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="7"/>
+      <c r="E27" s="9"/>
       <c r="F27" s="2"/>
-      <c r="G27" s="7"/>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="12"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="11"/>
       <c r="D28" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="E28" s="7"/>
+      <c r="E28" s="9"/>
       <c r="F28" s="2"/>
-      <c r="G28" s="7"/>
+      <c r="G28" s="9"/>
     </row>
     <row r="29" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="10"/>
+      <c r="B29" s="6"/>
       <c r="C29" s="13"/>
       <c r="D29" s="3"/>
-      <c r="E29" s="8"/>
+      <c r="E29" s="10"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="8"/>
+      <c r="G29" s="10"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B36" s="16" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B37" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="C19:C29"/>
     <mergeCell ref="E19:E29"/>
     <mergeCell ref="G19:G29"/>
+    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>